<commit_message>
Added mobile view for portal
</commit_message>
<xml_diff>
--- a/Server/wwwroot/Templates/PayslipTemplate.xlsx
+++ b/Server/wwwroot/Templates/PayslipTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboado\source\repos\NCMS-wasm\Server\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF02E12B-6091-467D-9D48-D1D67DDFD07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880"/>
+    <workbookView xWindow="-60" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,7 +106,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -386,19 +387,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>